<commit_message>
All bulk data uploaded, unit table fixed.
</commit_message>
<xml_diff>
--- a/mySQL_Create/data.xlsx
+++ b/mySQL_Create/data.xlsx
@@ -677,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -989,7 +989,7 @@
         <v>63</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>

</xml_diff>